<commit_message>
Updated Wiring, Pricing Details
Added pin numbers for RPI wiring, added materials costs for platform
pricing. Price remains below $2000.
</commit_message>
<xml_diff>
--- a/Design+Setup Notes/Platform Pricing.xlsx
+++ b/Design+Setup Notes/Platform Pricing.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18528"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="144">
   <si>
     <t>Items</t>
   </si>
@@ -140,9 +140,6 @@
     <t>Total Cost:</t>
   </si>
   <si>
-    <t>E6C2-CWZ3E, 2000P/R</t>
-  </si>
-  <si>
     <t>https://www.sparkfun.com/products/11102</t>
   </si>
   <si>
@@ -164,12 +161,6 @@
     <t>For USB connectivity</t>
   </si>
   <si>
-    <t>https://www.mouser.com/ProductDetail/SparkFun-Electronics/WRL-11373/</t>
-  </si>
-  <si>
-    <t>For microcomputer connectivity</t>
-  </si>
-  <si>
     <t>https://www.sparkfun.com/products/11812</t>
   </si>
   <si>
@@ -308,9 +299,6 @@
     <t>Hammers.</t>
   </si>
   <si>
-    <t>Vitally Important.</t>
-  </si>
-  <si>
     <t>Tape Measures, Squares, etc.</t>
   </si>
   <si>
@@ -326,15 +314,6 @@
     <t>250lb load capacity</t>
   </si>
   <si>
-    <t>Mini USB-USBA Cable</t>
-  </si>
-  <si>
-    <t>USBB-USBA Cable</t>
-  </si>
-  <si>
-    <t>24V-9V Converter</t>
-  </si>
-  <si>
     <t>Insulated 22-Gauge Wire</t>
   </si>
   <si>
@@ -344,13 +323,139 @@
     <t>For motor/battery circuitry</t>
   </si>
   <si>
-    <t>For arduino/encoder circuity</t>
-  </si>
-  <si>
-    <t>For connection to Xbee Explorer</t>
-  </si>
-  <si>
-    <t>For connection to Arduino</t>
+    <t>Mini USB cables</t>
+  </si>
+  <si>
+    <t>USB 2 A-Male to Mini-B</t>
+  </si>
+  <si>
+    <t>Recommend at least 3 feet.</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/AmazonBasics-USB-2-0-Cable-Male/dp/B00NH13S44</t>
+  </si>
+  <si>
+    <t>47 uF Capacitors</t>
+  </si>
+  <si>
+    <t>.1 uF Capacitors</t>
+  </si>
+  <si>
+    <t>50V Radial</t>
+  </si>
+  <si>
+    <t>You only need 2, but 10 is cheaper.</t>
+  </si>
+  <si>
+    <t>https://www.jameco.com/z/R47-50-47uF-50V-Radial-Electrolytic-Capacitor-plusmn-20-37-_31114.html</t>
+  </si>
+  <si>
+    <t>Ceramic Disc</t>
+  </si>
+  <si>
+    <t>https://www.jameco.com/z/DC-01-Ceramic-Disc-Capacitor-0-01-micro-F-50V-plusmn-20-37-Z5U_15229.html</t>
+  </si>
+  <si>
+    <t>Soldering Iron</t>
+  </si>
+  <si>
+    <t>For circuitry.</t>
+  </si>
+  <si>
+    <t>For adjustments.</t>
+  </si>
+  <si>
+    <t>Any PCB is acceptable.</t>
+  </si>
+  <si>
+    <t>Don't use breadboards - use soldering.</t>
+  </si>
+  <si>
+    <t>Prototyping Circuit Boards</t>
+  </si>
+  <si>
+    <t>https://www.jameco.com/z/SB400-Busboard-Prototype-Systems-SB400-Solderable-PC-Breadboard-1-Sided-PCB-Matches-400-Tie-Point-Breadboards-With-Power-Rails_2125051.html</t>
+  </si>
+  <si>
+    <t>Specs available at link.</t>
+  </si>
+  <si>
+    <t>~$90 for 1x1 steel</t>
+  </si>
+  <si>
+    <t>~$20 for 1x4 steel</t>
+  </si>
+  <si>
+    <t>~$80 for steel plate</t>
+  </si>
+  <si>
+    <t>All metals were purchased locally.</t>
+  </si>
+  <si>
+    <t>Prices will vary.</t>
+  </si>
+  <si>
+    <t>~$20 for plywood</t>
+  </si>
+  <si>
+    <t>~$20 for MDF board</t>
+  </si>
+  <si>
+    <t>Use plywood scraps</t>
+  </si>
+  <si>
+    <t>24V-5V Converter</t>
+  </si>
+  <si>
+    <t>To power Raspberry Pi</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/Magnolian-Converter-Regulator-Supplies-Transformer/dp/B00BWLP88A</t>
+  </si>
+  <si>
+    <t>For RPi/encoder circuity</t>
+  </si>
+  <si>
+    <t>For connecting to RPi pins</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/dp/B00W8YDCGA/ref=asc_df_B00W8YDCGA5328701</t>
+  </si>
+  <si>
+    <t>40 22-Gauge Jumper Wires</t>
+  </si>
+  <si>
+    <t>Wire Strippers</t>
+  </si>
+  <si>
+    <t>For stripping wires.</t>
+  </si>
+  <si>
+    <t>(I actually used the sharp part of the pliers, don't tell Chris)</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/StrivedayTMFlexible-Silicone-Electric-electronic-electrics/dp/B01LH1FR6M/</t>
+  </si>
+  <si>
+    <t>Excess</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/GAUGE-GROUND-PRIMARY-STRANDED-COPPER/dp/B01AO1K5HW/</t>
+  </si>
+  <si>
+    <t>Total Materials Cost:</t>
+  </si>
+  <si>
+    <t>~$15</t>
+  </si>
+  <si>
+    <t>~$20</t>
+  </si>
+  <si>
+    <t>Total Cost incl. Materials:</t>
+  </si>
+  <si>
+    <t>E6C2-CWZ3E, 1024P/R</t>
   </si>
 </sst>
 </file>
@@ -752,10 +857,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F8B9D088-EB7F-4F3E-AC27-71CC733A0939}">
-  <dimension ref="A1:I52"/>
+  <dimension ref="A1:I57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="A45" sqref="A45:B52"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -784,10 +889,10 @@
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>1</v>
@@ -817,10 +922,10 @@
         <v>108</v>
       </c>
       <c r="F4" s="10" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="G4" s="10" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="H4" s="9" t="s">
         <v>5</v>
@@ -844,10 +949,10 @@
         <v>61.32</v>
       </c>
       <c r="F5" s="10" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="G5" s="10" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="H5" s="7" t="s">
         <v>6</v>
@@ -871,10 +976,10 @@
         <v>47.12</v>
       </c>
       <c r="F6" s="10" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="G6" s="10" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="H6" s="4" t="s">
         <v>7</v>
@@ -898,10 +1003,10 @@
         <v>15.6</v>
       </c>
       <c r="F7" s="10" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="G7" s="10" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="H7" s="7" t="s">
         <v>9</v>
@@ -925,10 +1030,10 @@
         <v>42.4</v>
       </c>
       <c r="F8" s="10" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="G8" s="10" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="H8" s="4" t="s">
         <v>24</v>
@@ -952,10 +1057,10 @@
         <v>1.1599999999999999</v>
       </c>
       <c r="F9" s="10" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="G9" s="10" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="H9" s="7" t="s">
         <v>10</v>
@@ -965,6 +1070,9 @@
       <c r="A10" s="3" t="s">
         <v>25</v>
       </c>
+      <c r="B10" s="3" t="s">
+        <v>117</v>
+      </c>
       <c r="C10" s="10">
         <v>289</v>
       </c>
@@ -976,10 +1084,10 @@
         <v>578</v>
       </c>
       <c r="F10" s="10" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="G10" s="10" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="H10" s="8" t="s">
         <v>8</v>
@@ -987,10 +1095,10 @@
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="C11" s="6">
         <v>13.92</v>
@@ -1003,13 +1111,13 @@
         <v>55.68</v>
       </c>
       <c r="F11" s="10" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="G11" s="10" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="H11" s="4" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
@@ -1033,7 +1141,7 @@
         <v>27</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>38</v>
+        <v>143</v>
       </c>
       <c r="C15" s="10">
         <v>39.950000000000003</v>
@@ -1042,17 +1150,17 @@
         <v>2</v>
       </c>
       <c r="E15" s="10">
-        <f t="shared" ref="E15:E19" si="1">PRODUCT(C15:D15)</f>
+        <f t="shared" ref="E15:E18" si="1">PRODUCT(C15:D15)</f>
         <v>79.900000000000006</v>
       </c>
       <c r="F15" s="10" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="G15" s="10" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="H15" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
@@ -1073,10 +1181,10 @@
         <v>7.59</v>
       </c>
       <c r="F16" s="10" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="G16" s="10" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="H16" s="4" t="s">
         <v>30</v>
@@ -1100,10 +1208,10 @@
         <v>57.87</v>
       </c>
       <c r="F17" s="10" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="G17" s="10" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="H17" s="4" t="s">
         <v>31</v>
@@ -1111,83 +1219,83 @@
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B18" s="3" t="s">
         <v>44</v>
-      </c>
-      <c r="B18" s="3" t="s">
-        <v>45</v>
       </c>
       <c r="C18" s="10">
         <v>24.95</v>
       </c>
       <c r="D18" s="3">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E18" s="10">
         <f t="shared" si="1"/>
-        <v>24.95</v>
+        <v>74.849999999999994</v>
       </c>
       <c r="F18" s="10" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="G18" s="10" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="H18" s="4" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="C19" s="10">
-        <v>9.9499999999999993</v>
+        <v>119.99</v>
       </c>
       <c r="D19" s="3">
         <v>2</v>
       </c>
       <c r="E19" s="10">
-        <f t="shared" si="1"/>
-        <v>19.899999999999999</v>
+        <f>PRODUCT(C19:D19)</f>
+        <v>239.98</v>
       </c>
       <c r="F19" s="10" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="G19" s="10" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="H19" s="4" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>42</v>
+        <v>50</v>
       </c>
       <c r="C20" s="10">
-        <v>119.99</v>
+        <v>40.97</v>
       </c>
       <c r="D20" s="3">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E20" s="10">
         <f>PRODUCT(C20:D20)</f>
-        <v>239.98</v>
+        <v>163.88</v>
       </c>
       <c r="F20" s="10" t="s">
-        <v>50</v>
+        <v>61</v>
       </c>
       <c r="G20" s="10" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="H20" s="4" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
@@ -1195,277 +1303,470 @@
         <v>49</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C21" s="10">
-        <v>40.97</v>
+        <v>64.989999999999995</v>
       </c>
       <c r="D21" s="3">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E21" s="10">
         <f>PRODUCT(C21:D21)</f>
-        <v>163.88</v>
+        <v>129.97999999999999</v>
       </c>
       <c r="F21" s="10" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="G21" s="10" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="H21" s="4" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
-        <v>52</v>
+        <v>99</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>54</v>
+        <v>100</v>
       </c>
       <c r="C22" s="10">
-        <v>64.989999999999995</v>
+        <v>4.79</v>
       </c>
       <c r="D22" s="3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E22" s="10">
         <f>PRODUCT(C22:D22)</f>
-        <v>129.97999999999999</v>
+        <v>14.370000000000001</v>
       </c>
       <c r="F22" s="10" t="s">
-        <v>64</v>
+        <v>47</v>
       </c>
       <c r="G22" s="10" t="s">
-        <v>63</v>
+        <v>101</v>
       </c>
       <c r="H22" s="4" t="s">
-        <v>55</v>
+        <v>102</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
-        <v>36</v>
+        <v>103</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="C23" s="10">
+        <v>0.15</v>
+      </c>
+      <c r="D23" s="3">
+        <v>10</v>
       </c>
       <c r="E23" s="10">
-        <f>SUM(E15:E22)</f>
-        <v>724.05</v>
-      </c>
-      <c r="F23" s="10"/>
-      <c r="G23" s="10"/>
+        <f>PRODUCT(C23:D23)</f>
+        <v>1.5</v>
+      </c>
+      <c r="F23" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="G23" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="H23" s="4" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="C24" s="10">
+        <v>0.12</v>
+      </c>
+      <c r="D24" s="3">
+        <v>10</v>
+      </c>
+      <c r="E24" s="10">
+        <f>PRODUCT(C24:D24)</f>
+        <v>1.2</v>
+      </c>
+      <c r="F24" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="G24" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="H24" s="4" t="s">
+        <v>109</v>
+      </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
-        <v>37</v>
+        <v>115</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="C25" s="10">
+        <v>4.95</v>
+      </c>
+      <c r="D25" s="3">
+        <v>2</v>
       </c>
       <c r="E25" s="10">
-        <f>SUM(E12,E23)</f>
-        <v>1633.33</v>
-      </c>
-      <c r="F25" s="3" t="s">
-        <v>40</v>
+        <f>PRODUCT(C25:D25)</f>
+        <v>9.9</v>
+      </c>
+      <c r="F25" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="G25" s="10" t="s">
+        <v>114</v>
+      </c>
+      <c r="H25" s="4" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A26" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="C26" s="10">
+        <v>7.98</v>
+      </c>
+      <c r="D26" s="3">
+        <v>2</v>
+      </c>
+      <c r="E26" s="10">
+        <f>PRODUCT(C26:D26)</f>
+        <v>15.96</v>
+      </c>
+      <c r="F26" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="G26" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="H26" s="4" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
-        <v>65</v>
+        <v>132</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="C27" s="10">
+        <v>6.41</v>
+      </c>
+      <c r="D27" s="3">
+        <v>1</v>
+      </c>
+      <c r="E27" s="10">
+        <f>PRODUCT(C27:D27)</f>
+        <v>6.41</v>
+      </c>
+      <c r="F27" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="G27" s="10"/>
+      <c r="H27" s="4" t="s">
+        <v>131</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="B28" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="D28" s="3">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A29" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="D29" s="3">
-        <v>4</v>
-      </c>
+        <v>36</v>
+      </c>
+      <c r="E28" s="10">
+        <f>SUM(E15:E27)</f>
+        <v>803.39</v>
+      </c>
+      <c r="F28" s="10"/>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="D30" s="3">
-        <v>8</v>
+        <v>37</v>
+      </c>
+      <c r="E30" s="10">
+        <f>SUM(E12,E28)</f>
+        <v>1712.67</v>
+      </c>
+      <c r="F30" s="3" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="D31" s="3">
+        <v>142</v>
+      </c>
+      <c r="E31" s="10">
+        <f>SUM(E30,E46)</f>
+        <v>1977.67</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A33" s="3" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A34" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="B34" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="D34" s="3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A35" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="D35" s="3">
         <v>4</v>
       </c>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A32" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="D32" s="3">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="D33" s="3">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="B34" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="D34" s="3">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="B35" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="D35" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="H35" s="4"/>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="B36" s="3" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="D36" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+      <c r="G36" s="3" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="B37" s="3" t="s">
-        <v>98</v>
+        <v>77</v>
       </c>
       <c r="D37" s="3">
         <v>4</v>
       </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E37" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="G37" s="3" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="B38" s="3" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+        <v>78</v>
+      </c>
+      <c r="D38" s="3">
+        <v>4</v>
+      </c>
+      <c r="E38" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="G38" s="3" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
-        <v>101</v>
-      </c>
-      <c r="B39" s="3" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+        <v>64</v>
+      </c>
+      <c r="D39" s="3">
+        <v>2</v>
+      </c>
+      <c r="E39" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="G39" s="3" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="s">
-        <v>103</v>
+        <v>65</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+        <v>66</v>
+      </c>
+      <c r="D40" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
-        <v>102</v>
+        <v>67</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+        <v>68</v>
+      </c>
+      <c r="D41" s="3">
+        <v>1</v>
+      </c>
+      <c r="E41" s="3" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" s="3" t="s">
-        <v>104</v>
+        <v>70</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+        <v>69</v>
+      </c>
+      <c r="D42" s="3">
+        <v>1</v>
+      </c>
+      <c r="E42" s="3" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A43" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="B43" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="D43" s="3">
+        <v>4</v>
+      </c>
+      <c r="E43" s="3" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A44" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="B44" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="D44" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="E44" s="10" t="s">
+        <v>141</v>
+      </c>
+      <c r="H44" s="4" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="B45" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="D45" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="E45" s="10" t="s">
+        <v>140</v>
+      </c>
+      <c r="H45" s="4" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A46" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="E46" s="6">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A48" s="3" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="B49" s="3" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A50" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="B50" s="3" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A51" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="B51" s="3" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46" s="3" t="s">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A52" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="B52" s="3" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A53" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="B53" s="3" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A54" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="B46" s="3" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A47" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="B47" s="3" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A48" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="B48" s="3" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A49" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="B49" s="3" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A50" s="3" t="s">
+      <c r="B54" s="3" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A55" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="B50" s="3" t="s">
+      <c r="B55" s="3" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A51" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="B51" s="3" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A52" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="B52" s="3" t="s">
-        <v>96</v>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A56" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="B56" s="3" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A57" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="B57" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="C57" s="3" t="s">
+        <v>135</v>
       </c>
     </row>
   </sheetData>
@@ -1480,14 +1781,20 @@
     <hyperlink ref="H16" r:id="rId8" display="https://www.newegg.com/Product/Product.aspx?Item=9SIAAZM4CV8189&amp;ignorebbr=1&amp;nm_mc=KNC-GoogleMKP-PC&amp;cm_mmc=KNC-GoogleMKP-PC-_-pla-_-EC+-+Test+%26+Measurement-_-9SIAAZM4CV8189&amp;gclid=CjwKCAjwmK3OBRBKEiwAOL6t1Gm-EIm2mMBs8TutN7YNg1TSPTops_dD4QtmQN_jf9KvjcITUM2NVxoCXMEQAvD_BwE&amp;gclsrc=aw.ds" xr:uid="{4F29CBBC-C984-4A0F-9FF8-7AC6D07EF2FC}"/>
     <hyperlink ref="H17" r:id="rId9" xr:uid="{9B8C5C33-7829-4795-9390-96C1C4836892}"/>
     <hyperlink ref="H15" r:id="rId10" xr:uid="{256BAD20-B5C2-4B74-BA2F-1F2C76781276}"/>
-    <hyperlink ref="H19" r:id="rId11" xr:uid="{94A0EF0E-6032-425F-8A65-66C1845DBC35}"/>
-    <hyperlink ref="H20" r:id="rId12" xr:uid="{48943A3B-4EC6-471A-B0AE-5DC2524A5F0F}"/>
-    <hyperlink ref="H21" r:id="rId13" xr:uid="{372168C7-D476-451B-8125-1AD4D9977E26}"/>
-    <hyperlink ref="H22" r:id="rId14" xr:uid="{B09BB86E-A73E-4E09-8C0A-E5FC9684E3E4}"/>
-    <hyperlink ref="H18" r:id="rId15" xr:uid="{B7B9D5CB-9CDC-4D0B-A18E-CF4B64A9C145}"/>
-    <hyperlink ref="H11" r:id="rId16" xr:uid="{DC9BFAC3-F11F-4E0B-A1A4-C404372ADAB8}"/>
+    <hyperlink ref="H19" r:id="rId11" xr:uid="{48943A3B-4EC6-471A-B0AE-5DC2524A5F0F}"/>
+    <hyperlink ref="H20" r:id="rId12" xr:uid="{372168C7-D476-451B-8125-1AD4D9977E26}"/>
+    <hyperlink ref="H21" r:id="rId13" xr:uid="{B09BB86E-A73E-4E09-8C0A-E5FC9684E3E4}"/>
+    <hyperlink ref="H18" r:id="rId14" xr:uid="{B7B9D5CB-9CDC-4D0B-A18E-CF4B64A9C145}"/>
+    <hyperlink ref="H11" r:id="rId15" xr:uid="{DC9BFAC3-F11F-4E0B-A1A4-C404372ADAB8}"/>
+    <hyperlink ref="H22" r:id="rId16" xr:uid="{AF10B725-21C8-40EE-B2FC-CD9A14DAA7CD}"/>
+    <hyperlink ref="H23" r:id="rId17" xr:uid="{3FDA7518-6146-4772-9C84-53BFA5E8B4F9}"/>
+    <hyperlink ref="H24" r:id="rId18" xr:uid="{17B839ED-63EF-46C4-AF3B-1E1A54DE8DEF}"/>
+    <hyperlink ref="H26" r:id="rId19" xr:uid="{444B920E-8D64-4C60-ABA6-B785BACBC070}"/>
+    <hyperlink ref="H27" r:id="rId20" xr:uid="{D43F79F7-B56A-44A6-87FC-892FBBCB9A90}"/>
+    <hyperlink ref="H44" r:id="rId21" xr:uid="{AC4DA7E7-CE31-4066-ADF0-82D96A6640B1}"/>
+    <hyperlink ref="H45" r:id="rId22" xr:uid="{C7358071-0BB2-488D-9872-512647880368}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId17"/>
+  <pageSetup orientation="portrait" r:id="rId23"/>
 </worksheet>
 </file>
</xml_diff>